<commit_message>
Test cases exported from Test Rail updated.
</commit_message>
<xml_diff>
--- a/testing/reports/test-cases/mg_fg_movie_shop_backend.xlsx
+++ b/testing/reports/test-cases/mg_fg_movie_shop_backend.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="355">
   <si>
     <t>ID</t>
   </si>
@@ -79,7 +79,7 @@
     <t>C34</t>
   </si>
   <si>
-    <t>Read movie by id with existing id</t>
+    <t>Read movie by id with existing {movie_id}</t>
   </si>
   <si>
     <t xml:space="preserve">Status: 200 Ok
@@ -159,22 +159,6 @@
   <si>
     <t xml:space="preserve">Do a GET request to /movies/{movie_id} without a movie id
 </t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>Read movie by id with existing {movie_id}</t>
-  </si>
-  <si>
-    <t>Status: 200 OK
-Return a movie with a valid structure.</t>
-  </si>
-  <si>
-    <t>There is at least one movie created.</t>
-  </si>
-  <si>
-    <t>Do a GET request to /movies{movie_id} with an existing movie id.</t>
   </si>
   <si>
     <t>C8</t>
@@ -1524,7 +1508,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G94"/>
+  <dimension ref="A1:G93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1767,13 +1751,13 @@
         <v>51</v>
       </c>
       <c r="D11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" t="s">
         <v>52</v>
-      </c>
-      <c r="E11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" t="s">
-        <v>53</v>
       </c>
       <c r="G11" t="s">
         <v>13</v>
@@ -1781,22 +1765,22 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" t="s">
         <v>54</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>55</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" t="s">
         <v>56</v>
-      </c>
-      <c r="D12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" t="s">
-        <v>57</v>
       </c>
       <c r="G12" t="s">
         <v>13</v>
@@ -1804,16 +1788,16 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" t="s">
         <v>58</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>59</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>60</v>
-      </c>
-      <c r="D13" t="s">
-        <v>35</v>
       </c>
       <c r="E13" t="s">
         <v>11</v>
@@ -1836,13 +1820,13 @@
         <v>64</v>
       </c>
       <c r="D14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" t="s">
         <v>65</v>
-      </c>
-      <c r="E14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" t="s">
-        <v>66</v>
       </c>
       <c r="G14" t="s">
         <v>13</v>
@@ -1850,22 +1834,22 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" t="s">
         <v>67</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" t="s">
         <v>68</v>
       </c>
-      <c r="C15" t="s">
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" t="s">
         <v>69</v>
-      </c>
-      <c r="D15" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" t="s">
-        <v>70</v>
       </c>
       <c r="G15" t="s">
         <v>13</v>
@@ -1873,22 +1857,22 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" t="s">
         <v>71</v>
-      </c>
-      <c r="B16" t="s">
-        <v>72</v>
       </c>
       <c r="C16" t="s">
         <v>34</v>
       </c>
       <c r="D16" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" t="s">
         <v>73</v>
-      </c>
-      <c r="E16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" t="s">
-        <v>74</v>
       </c>
       <c r="G16" t="s">
         <v>13</v>
@@ -1896,22 +1880,22 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" t="s">
         <v>75</v>
-      </c>
-      <c r="B17" t="s">
-        <v>76</v>
       </c>
       <c r="C17" t="s">
         <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E17" t="s">
         <v>11</v>
       </c>
       <c r="F17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G17" t="s">
         <v>13</v>
@@ -1919,22 +1903,22 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C18" t="s">
         <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E18" t="s">
         <v>11</v>
       </c>
       <c r="F18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G18" t="s">
         <v>13</v>
@@ -1942,22 +1926,22 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B19" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C19" t="s">
         <v>34</v>
       </c>
       <c r="D19" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="E19" t="s">
         <v>11</v>
       </c>
       <c r="F19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G19" t="s">
         <v>13</v>
@@ -1965,22 +1949,22 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" t="s">
         <v>85</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>86</v>
       </c>
-      <c r="C20" t="s">
-        <v>34</v>
-      </c>
       <c r="D20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" t="s">
         <v>87</v>
-      </c>
-      <c r="E20" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" t="s">
-        <v>88</v>
       </c>
       <c r="G20" t="s">
         <v>13</v>
@@ -1988,22 +1972,22 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" t="s">
         <v>89</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>90</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" t="s">
         <v>91</v>
-      </c>
-      <c r="D21" t="s">
-        <v>77</v>
-      </c>
-      <c r="E21" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" t="s">
-        <v>92</v>
       </c>
       <c r="G21" t="s">
         <v>13</v>
@@ -2011,22 +1995,19 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22" t="s">
         <v>93</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
+        <v>86</v>
+      </c>
+      <c r="E22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" t="s">
         <v>94</v>
-      </c>
-      <c r="C22" t="s">
-        <v>95</v>
-      </c>
-      <c r="D22" t="s">
-        <v>77</v>
-      </c>
-      <c r="E22" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" t="s">
-        <v>96</v>
       </c>
       <c r="G22" t="s">
         <v>13</v>
@@ -2034,19 +2015,19 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" t="s">
         <v>97</v>
-      </c>
-      <c r="B23" t="s">
-        <v>98</v>
-      </c>
-      <c r="C23" t="s">
-        <v>91</v>
-      </c>
-      <c r="E23" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" t="s">
-        <v>99</v>
       </c>
       <c r="G23" t="s">
         <v>13</v>
@@ -2054,13 +2035,16 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
+        <v>98</v>
+      </c>
+      <c r="B24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" t="s">
         <v>100</v>
       </c>
-      <c r="B24" t="s">
+      <c r="D24" t="s">
         <v>101</v>
-      </c>
-      <c r="C24" t="s">
-        <v>34</v>
       </c>
       <c r="E24" t="s">
         <v>11</v>
@@ -2106,13 +2090,13 @@
         <v>110</v>
       </c>
       <c r="D26" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" t="s">
         <v>111</v>
-      </c>
-      <c r="E26" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26" t="s">
-        <v>112</v>
       </c>
       <c r="G26" t="s">
         <v>13</v>
@@ -2120,22 +2104,22 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
+        <v>112</v>
+      </c>
+      <c r="B27" t="s">
         <v>113</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" t="s">
+        <v>68</v>
+      </c>
+      <c r="E27" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" t="s">
         <v>114</v>
-      </c>
-      <c r="C27" t="s">
-        <v>115</v>
-      </c>
-      <c r="D27" t="s">
-        <v>26</v>
-      </c>
-      <c r="E27" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27" t="s">
-        <v>116</v>
       </c>
       <c r="G27" t="s">
         <v>13</v>
@@ -2143,16 +2127,16 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
+        <v>115</v>
+      </c>
+      <c r="B28" t="s">
+        <v>116</v>
+      </c>
+      <c r="C28" t="s">
         <v>117</v>
       </c>
-      <c r="B28" t="s">
+      <c r="D28" t="s">
         <v>118</v>
-      </c>
-      <c r="C28" t="s">
-        <v>34</v>
-      </c>
-      <c r="D28" t="s">
-        <v>73</v>
       </c>
       <c r="E28" t="s">
         <v>11</v>
@@ -2181,7 +2165,7 @@
         <v>11</v>
       </c>
       <c r="F29" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G29" t="s">
         <v>13</v>
@@ -2189,22 +2173,22 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
+        <v>124</v>
+      </c>
+      <c r="B30" t="s">
         <v>125</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
+        <v>105</v>
+      </c>
+      <c r="D30" t="s">
         <v>126</v>
       </c>
-      <c r="C30" t="s">
-        <v>127</v>
-      </c>
-      <c r="D30" t="s">
-        <v>128</v>
-      </c>
       <c r="E30" t="s">
         <v>11</v>
       </c>
       <c r="F30" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G30" t="s">
         <v>13</v>
@@ -2212,22 +2196,22 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
+        <v>127</v>
+      </c>
+      <c r="B31" t="s">
+        <v>128</v>
+      </c>
+      <c r="C31" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" t="s">
         <v>129</v>
-      </c>
-      <c r="B31" t="s">
-        <v>130</v>
-      </c>
-      <c r="C31" t="s">
-        <v>110</v>
-      </c>
-      <c r="D31" t="s">
-        <v>131</v>
-      </c>
-      <c r="E31" t="s">
-        <v>11</v>
-      </c>
-      <c r="F31" t="s">
-        <v>124</v>
       </c>
       <c r="G31" t="s">
         <v>13</v>
@@ -2235,22 +2219,22 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
+        <v>130</v>
+      </c>
+      <c r="B32" t="s">
+        <v>131</v>
+      </c>
+      <c r="C32" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32" t="s">
+        <v>68</v>
+      </c>
+      <c r="E32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" t="s">
         <v>132</v>
-      </c>
-      <c r="B32" t="s">
-        <v>133</v>
-      </c>
-      <c r="C32" t="s">
-        <v>25</v>
-      </c>
-      <c r="D32" t="s">
-        <v>26</v>
-      </c>
-      <c r="E32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F32" t="s">
-        <v>134</v>
       </c>
       <c r="G32" t="s">
         <v>13</v>
@@ -2258,22 +2242,22 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
+        <v>133</v>
+      </c>
+      <c r="B33" t="s">
+        <v>134</v>
+      </c>
+      <c r="C33" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" t="s">
+        <v>118</v>
+      </c>
+      <c r="E33" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" t="s">
         <v>135</v>
-      </c>
-      <c r="B33" t="s">
-        <v>136</v>
-      </c>
-      <c r="C33" t="s">
-        <v>34</v>
-      </c>
-      <c r="D33" t="s">
-        <v>73</v>
-      </c>
-      <c r="E33" t="s">
-        <v>11</v>
-      </c>
-      <c r="F33" t="s">
-        <v>137</v>
       </c>
       <c r="G33" t="s">
         <v>13</v>
@@ -2281,16 +2265,16 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
+        <v>136</v>
+      </c>
+      <c r="B34" t="s">
+        <v>137</v>
+      </c>
+      <c r="C34" t="s">
         <v>138</v>
       </c>
-      <c r="B34" t="s">
+      <c r="D34" t="s">
         <v>139</v>
-      </c>
-      <c r="C34" t="s">
-        <v>21</v>
-      </c>
-      <c r="D34" t="s">
-        <v>123</v>
       </c>
       <c r="E34" t="s">
         <v>11</v>
@@ -2310,16 +2294,16 @@
         <v>142</v>
       </c>
       <c r="C35" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" t="s">
         <v>143</v>
-      </c>
-      <c r="D35" t="s">
-        <v>144</v>
-      </c>
-      <c r="E35" t="s">
-        <v>11</v>
-      </c>
-      <c r="F35" t="s">
-        <v>145</v>
       </c>
       <c r="G35" t="s">
         <v>13</v>
@@ -2327,16 +2311,16 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
+        <v>144</v>
+      </c>
+      <c r="B36" t="s">
+        <v>145</v>
+      </c>
+      <c r="C36" t="s">
         <v>146</v>
       </c>
-      <c r="B36" t="s">
+      <c r="D36" t="s">
         <v>147</v>
-      </c>
-      <c r="C36" t="s">
-        <v>25</v>
-      </c>
-      <c r="D36" t="s">
-        <v>26</v>
       </c>
       <c r="E36" t="s">
         <v>11</v>
@@ -2356,16 +2340,16 @@
         <v>150</v>
       </c>
       <c r="C37" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" t="s">
         <v>151</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" t="s">
         <v>152</v>
-      </c>
-      <c r="E37" t="s">
-        <v>11</v>
-      </c>
-      <c r="F37" t="s">
-        <v>153</v>
       </c>
       <c r="G37" t="s">
         <v>13</v>
@@ -2373,22 +2357,22 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
+        <v>153</v>
+      </c>
+      <c r="B38" t="s">
         <v>154</v>
-      </c>
-      <c r="B38" t="s">
-        <v>155</v>
       </c>
       <c r="C38" t="s">
         <v>25</v>
       </c>
       <c r="D38" t="s">
+        <v>155</v>
+      </c>
+      <c r="E38" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" t="s">
         <v>156</v>
-      </c>
-      <c r="E38" t="s">
-        <v>11</v>
-      </c>
-      <c r="F38" t="s">
-        <v>157</v>
       </c>
       <c r="G38" t="s">
         <v>13</v>
@@ -2396,13 +2380,13 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
+        <v>157</v>
+      </c>
+      <c r="B39" t="s">
         <v>158</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>159</v>
-      </c>
-      <c r="C39" t="s">
-        <v>25</v>
       </c>
       <c r="D39" t="s">
         <v>160</v>
@@ -2425,16 +2409,16 @@
         <v>163</v>
       </c>
       <c r="C40" t="s">
+        <v>138</v>
+      </c>
+      <c r="D40" t="s">
+        <v>118</v>
+      </c>
+      <c r="E40" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" t="s">
         <v>164</v>
-      </c>
-      <c r="D40" t="s">
-        <v>165</v>
-      </c>
-      <c r="E40" t="s">
-        <v>11</v>
-      </c>
-      <c r="F40" t="s">
-        <v>166</v>
       </c>
       <c r="G40" t="s">
         <v>13</v>
@@ -2442,22 +2426,22 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
+        <v>165</v>
+      </c>
+      <c r="B41" t="s">
+        <v>166</v>
+      </c>
+      <c r="C41" t="s">
+        <v>51</v>
+      </c>
+      <c r="D41" t="s">
+        <v>26</v>
+      </c>
+      <c r="E41" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" t="s">
         <v>167</v>
-      </c>
-      <c r="B41" t="s">
-        <v>168</v>
-      </c>
-      <c r="C41" t="s">
-        <v>143</v>
-      </c>
-      <c r="D41" t="s">
-        <v>123</v>
-      </c>
-      <c r="E41" t="s">
-        <v>11</v>
-      </c>
-      <c r="F41" t="s">
-        <v>169</v>
       </c>
       <c r="G41" t="s">
         <v>13</v>
@@ -2465,22 +2449,22 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
+        <v>168</v>
+      </c>
+      <c r="B42" t="s">
+        <v>169</v>
+      </c>
+      <c r="C42" t="s">
         <v>170</v>
       </c>
-      <c r="B42" t="s">
+      <c r="D42" t="s">
+        <v>47</v>
+      </c>
+      <c r="E42" t="s">
+        <v>11</v>
+      </c>
+      <c r="F42" t="s">
         <v>171</v>
-      </c>
-      <c r="C42" t="s">
-        <v>56</v>
-      </c>
-      <c r="D42" t="s">
-        <v>26</v>
-      </c>
-      <c r="E42" t="s">
-        <v>11</v>
-      </c>
-      <c r="F42" t="s">
-        <v>172</v>
       </c>
       <c r="G42" t="s">
         <v>13</v>
@@ -2488,22 +2472,19 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
+        <v>172</v>
+      </c>
+      <c r="B43" t="s">
         <v>173</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
+        <v>25</v>
+      </c>
+      <c r="E43" t="s">
+        <v>11</v>
+      </c>
+      <c r="F43" t="s">
         <v>174</v>
-      </c>
-      <c r="C43" t="s">
-        <v>175</v>
-      </c>
-      <c r="D43" t="s">
-        <v>52</v>
-      </c>
-      <c r="E43" t="s">
-        <v>11</v>
-      </c>
-      <c r="F43" t="s">
-        <v>176</v>
       </c>
       <c r="G43" t="s">
         <v>13</v>
@@ -2511,19 +2492,22 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
+        <v>175</v>
+      </c>
+      <c r="B44" t="s">
+        <v>176</v>
+      </c>
+      <c r="C44" t="s">
+        <v>34</v>
+      </c>
+      <c r="D44" t="s">
         <v>177</v>
       </c>
-      <c r="B44" t="s">
+      <c r="E44" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" t="s">
         <v>178</v>
-      </c>
-      <c r="C44" t="s">
-        <v>25</v>
-      </c>
-      <c r="E44" t="s">
-        <v>11</v>
-      </c>
-      <c r="F44" t="s">
-        <v>179</v>
       </c>
       <c r="G44" t="s">
         <v>13</v>
@@ -2531,22 +2515,22 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
+        <v>179</v>
+      </c>
+      <c r="B45" t="s">
         <v>180</v>
-      </c>
-      <c r="B45" t="s">
-        <v>181</v>
       </c>
       <c r="C45" t="s">
         <v>34</v>
       </c>
       <c r="D45" t="s">
-        <v>182</v>
+        <v>47</v>
       </c>
       <c r="E45" t="s">
         <v>11</v>
       </c>
       <c r="F45" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G45" t="s">
         <v>13</v>
@@ -2554,22 +2538,19 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B46" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C46" t="s">
         <v>34</v>
       </c>
-      <c r="D46" t="s">
-        <v>52</v>
-      </c>
       <c r="E46" t="s">
         <v>11</v>
       </c>
       <c r="F46" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G46" t="s">
         <v>13</v>
@@ -2577,19 +2558,22 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B47" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C47" t="s">
         <v>34</v>
       </c>
+      <c r="D47" t="s">
+        <v>47</v>
+      </c>
       <c r="E47" t="s">
         <v>11</v>
       </c>
       <c r="F47" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G47" t="s">
         <v>13</v>
@@ -2597,16 +2581,16 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
+        <v>188</v>
+      </c>
+      <c r="B48" t="s">
+        <v>189</v>
+      </c>
+      <c r="C48" t="s">
         <v>190</v>
       </c>
-      <c r="B48" t="s">
+      <c r="D48" t="s">
         <v>191</v>
-      </c>
-      <c r="C48" t="s">
-        <v>34</v>
-      </c>
-      <c r="D48" t="s">
-        <v>52</v>
       </c>
       <c r="E48" t="s">
         <v>11</v>
@@ -2626,16 +2610,16 @@
         <v>194</v>
       </c>
       <c r="C49" t="s">
+        <v>34</v>
+      </c>
+      <c r="D49" t="s">
+        <v>47</v>
+      </c>
+      <c r="E49" t="s">
+        <v>11</v>
+      </c>
+      <c r="F49" t="s">
         <v>195</v>
-      </c>
-      <c r="D49" t="s">
-        <v>196</v>
-      </c>
-      <c r="E49" t="s">
-        <v>11</v>
-      </c>
-      <c r="F49" t="s">
-        <v>197</v>
       </c>
       <c r="G49" t="s">
         <v>13</v>
@@ -2643,22 +2627,22 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B50" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C50" t="s">
         <v>34</v>
       </c>
       <c r="D50" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E50" t="s">
         <v>11</v>
       </c>
       <c r="F50" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G50" t="s">
         <v>13</v>
@@ -2666,22 +2650,22 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
+        <v>199</v>
+      </c>
+      <c r="B51" t="s">
+        <v>200</v>
+      </c>
+      <c r="C51" t="s">
+        <v>25</v>
+      </c>
+      <c r="D51" t="s">
+        <v>47</v>
+      </c>
+      <c r="E51" t="s">
+        <v>11</v>
+      </c>
+      <c r="F51" t="s">
         <v>201</v>
-      </c>
-      <c r="B51" t="s">
-        <v>202</v>
-      </c>
-      <c r="C51" t="s">
-        <v>34</v>
-      </c>
-      <c r="D51" t="s">
-        <v>52</v>
-      </c>
-      <c r="E51" t="s">
-        <v>11</v>
-      </c>
-      <c r="F51" t="s">
-        <v>203</v>
       </c>
       <c r="G51" t="s">
         <v>13</v>
@@ -2689,16 +2673,16 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
+        <v>202</v>
+      </c>
+      <c r="B52" t="s">
+        <v>203</v>
+      </c>
+      <c r="C52" t="s">
         <v>204</v>
       </c>
-      <c r="B52" t="s">
+      <c r="D52" t="s">
         <v>205</v>
-      </c>
-      <c r="C52" t="s">
-        <v>25</v>
-      </c>
-      <c r="D52" t="s">
-        <v>52</v>
       </c>
       <c r="E52" t="s">
         <v>11</v>
@@ -2718,16 +2702,16 @@
         <v>208</v>
       </c>
       <c r="C53" t="s">
+        <v>204</v>
+      </c>
+      <c r="D53" t="s">
         <v>209</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E53" t="s">
+        <v>11</v>
+      </c>
+      <c r="F53" t="s">
         <v>210</v>
-      </c>
-      <c r="E53" t="s">
-        <v>11</v>
-      </c>
-      <c r="F53" t="s">
-        <v>211</v>
       </c>
       <c r="G53" t="s">
         <v>13</v>
@@ -2735,22 +2719,22 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" t="s">
+        <v>211</v>
+      </c>
+      <c r="B54" t="s">
         <v>212</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
         <v>213</v>
       </c>
-      <c r="C54" t="s">
-        <v>209</v>
-      </c>
       <c r="D54" t="s">
+        <v>10</v>
+      </c>
+      <c r="E54" t="s">
+        <v>11</v>
+      </c>
+      <c r="F54" t="s">
         <v>214</v>
-      </c>
-      <c r="E54" t="s">
-        <v>11</v>
-      </c>
-      <c r="F54" t="s">
-        <v>215</v>
       </c>
       <c r="G54" t="s">
         <v>13</v>
@@ -2758,22 +2742,19 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" t="s">
+        <v>215</v>
+      </c>
+      <c r="B55" t="s">
         <v>216</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
         <v>217</v>
       </c>
-      <c r="C55" t="s">
+      <c r="E55" t="s">
+        <v>11</v>
+      </c>
+      <c r="F55" t="s">
         <v>218</v>
-      </c>
-      <c r="D55" t="s">
-        <v>10</v>
-      </c>
-      <c r="E55" t="s">
-        <v>11</v>
-      </c>
-      <c r="F55" t="s">
-        <v>219</v>
       </c>
       <c r="G55" t="s">
         <v>13</v>
@@ -2781,12 +2762,15 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
+        <v>219</v>
+      </c>
+      <c r="B56" t="s">
         <v>220</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" t="s">
         <v>221</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>222</v>
       </c>
       <c r="E56" t="s">
@@ -2809,14 +2793,11 @@
       <c r="C57" t="s">
         <v>226</v>
       </c>
-      <c r="D57" t="s">
+      <c r="E57" t="s">
+        <v>11</v>
+      </c>
+      <c r="F57" t="s">
         <v>227</v>
-      </c>
-      <c r="E57" t="s">
-        <v>11</v>
-      </c>
-      <c r="F57" t="s">
-        <v>228</v>
       </c>
       <c r="G57" t="s">
         <v>13</v>
@@ -2824,19 +2805,22 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" t="s">
+        <v>228</v>
+      </c>
+      <c r="B58" t="s">
         <v>229</v>
       </c>
-      <c r="B58" t="s">
+      <c r="C58" t="s">
         <v>230</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" t="s">
+        <v>10</v>
+      </c>
+      <c r="E58" t="s">
+        <v>11</v>
+      </c>
+      <c r="F58" t="s">
         <v>231</v>
-      </c>
-      <c r="E58" t="s">
-        <v>11</v>
-      </c>
-      <c r="F58" t="s">
-        <v>232</v>
       </c>
       <c r="G58" t="s">
         <v>13</v>
@@ -2844,22 +2828,19 @@
     </row>
     <row r="59" spans="1:7">
       <c r="A59" t="s">
+        <v>232</v>
+      </c>
+      <c r="B59" t="s">
         <v>233</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" t="s">
+        <v>217</v>
+      </c>
+      <c r="E59" t="s">
+        <v>11</v>
+      </c>
+      <c r="F59" t="s">
         <v>234</v>
-      </c>
-      <c r="C59" t="s">
-        <v>235</v>
-      </c>
-      <c r="D59" t="s">
-        <v>10</v>
-      </c>
-      <c r="E59" t="s">
-        <v>11</v>
-      </c>
-      <c r="F59" t="s">
-        <v>236</v>
       </c>
       <c r="G59" t="s">
         <v>13</v>
@@ -2867,19 +2848,22 @@
     </row>
     <row r="60" spans="1:7">
       <c r="A60" t="s">
+        <v>235</v>
+      </c>
+      <c r="B60" t="s">
+        <v>236</v>
+      </c>
+      <c r="C60" t="s">
         <v>237</v>
       </c>
-      <c r="B60" t="s">
+      <c r="D60" t="s">
+        <v>222</v>
+      </c>
+      <c r="E60" t="s">
+        <v>11</v>
+      </c>
+      <c r="F60" t="s">
         <v>238</v>
-      </c>
-      <c r="C60" t="s">
-        <v>222</v>
-      </c>
-      <c r="E60" t="s">
-        <v>11</v>
-      </c>
-      <c r="F60" t="s">
-        <v>239</v>
       </c>
       <c r="G60" t="s">
         <v>13</v>
@@ -2887,22 +2871,19 @@
     </row>
     <row r="61" spans="1:7">
       <c r="A61" t="s">
+        <v>239</v>
+      </c>
+      <c r="B61" t="s">
         <v>240</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" t="s">
         <v>241</v>
       </c>
-      <c r="C61" t="s">
+      <c r="E61" t="s">
+        <v>11</v>
+      </c>
+      <c r="F61" t="s">
         <v>242</v>
-      </c>
-      <c r="D61" t="s">
-        <v>227</v>
-      </c>
-      <c r="E61" t="s">
-        <v>11</v>
-      </c>
-      <c r="F61" t="s">
-        <v>243</v>
       </c>
       <c r="G61" t="s">
         <v>13</v>
@@ -2910,19 +2891,22 @@
     </row>
     <row r="62" spans="1:7">
       <c r="A62" t="s">
+        <v>243</v>
+      </c>
+      <c r="B62" t="s">
         <v>244</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C62" t="s">
         <v>245</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
         <v>246</v>
       </c>
       <c r="E62" t="s">
-        <v>11</v>
+        <v>247</v>
       </c>
       <c r="F62" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="G62" t="s">
         <v>13</v>
@@ -2930,22 +2914,22 @@
     </row>
     <row r="63" spans="1:7">
       <c r="A63" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B63" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C63" t="s">
-        <v>250</v>
+        <v>217</v>
       </c>
       <c r="D63" t="s">
         <v>251</v>
       </c>
       <c r="E63" t="s">
+        <v>247</v>
+      </c>
+      <c r="F63" t="s">
         <v>252</v>
-      </c>
-      <c r="F63" t="s">
-        <v>253</v>
       </c>
       <c r="G63" t="s">
         <v>13</v>
@@ -2953,22 +2937,22 @@
     </row>
     <row r="64" spans="1:7">
       <c r="A64" t="s">
+        <v>253</v>
+      </c>
+      <c r="B64" t="s">
         <v>254</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" t="s">
         <v>255</v>
       </c>
-      <c r="C64" t="s">
-        <v>222</v>
-      </c>
       <c r="D64" t="s">
+        <v>26</v>
+      </c>
+      <c r="E64" t="s">
+        <v>247</v>
+      </c>
+      <c r="F64" t="s">
         <v>256</v>
-      </c>
-      <c r="E64" t="s">
-        <v>252</v>
-      </c>
-      <c r="F64" t="s">
-        <v>257</v>
       </c>
       <c r="G64" t="s">
         <v>13</v>
@@ -2976,22 +2960,22 @@
     </row>
     <row r="65" spans="1:7">
       <c r="A65" t="s">
+        <v>257</v>
+      </c>
+      <c r="B65" t="s">
         <v>258</v>
       </c>
-      <c r="B65" t="s">
-        <v>259</v>
-      </c>
       <c r="C65" t="s">
-        <v>260</v>
+        <v>34</v>
       </c>
       <c r="D65" t="s">
         <v>26</v>
       </c>
       <c r="E65" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="F65" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G65" t="s">
         <v>13</v>
@@ -2999,10 +2983,10 @@
     </row>
     <row r="66" spans="1:7">
       <c r="A66" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B66" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C66" t="s">
         <v>34</v>
@@ -3011,10 +2995,10 @@
         <v>26</v>
       </c>
       <c r="E66" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="F66" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G66" t="s">
         <v>13</v>
@@ -3022,10 +3006,10 @@
     </row>
     <row r="67" spans="1:7">
       <c r="A67" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B67" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C67" t="s">
         <v>34</v>
@@ -3034,10 +3018,10 @@
         <v>26</v>
       </c>
       <c r="E67" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="F67" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G67" t="s">
         <v>13</v>
@@ -3045,22 +3029,22 @@
     </row>
     <row r="68" spans="1:7">
       <c r="A68" t="s">
+        <v>266</v>
+      </c>
+      <c r="B68" t="s">
+        <v>267</v>
+      </c>
+      <c r="C68" t="s">
         <v>268</v>
-      </c>
-      <c r="B68" t="s">
-        <v>269</v>
-      </c>
-      <c r="C68" t="s">
-        <v>34</v>
       </c>
       <c r="D68" t="s">
         <v>26</v>
       </c>
       <c r="E68" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="F68" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G68" t="s">
         <v>13</v>
@@ -3068,22 +3052,22 @@
     </row>
     <row r="69" spans="1:7">
       <c r="A69" t="s">
+        <v>270</v>
+      </c>
+      <c r="B69" t="s">
         <v>271</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" t="s">
         <v>272</v>
       </c>
-      <c r="C69" t="s">
+      <c r="D69" t="s">
+        <v>246</v>
+      </c>
+      <c r="E69" t="s">
+        <v>247</v>
+      </c>
+      <c r="F69" t="s">
         <v>273</v>
-      </c>
-      <c r="D69" t="s">
-        <v>26</v>
-      </c>
-      <c r="E69" t="s">
-        <v>252</v>
-      </c>
-      <c r="F69" t="s">
-        <v>274</v>
       </c>
       <c r="G69" t="s">
         <v>13</v>
@@ -3091,22 +3075,22 @@
     </row>
     <row r="70" spans="1:7">
       <c r="A70" t="s">
+        <v>274</v>
+      </c>
+      <c r="B70" t="s">
         <v>275</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" t="s">
+        <v>64</v>
+      </c>
+      <c r="D70" t="s">
+        <v>26</v>
+      </c>
+      <c r="E70" t="s">
+        <v>247</v>
+      </c>
+      <c r="F70" t="s">
         <v>276</v>
-      </c>
-      <c r="C70" t="s">
-        <v>277</v>
-      </c>
-      <c r="D70" t="s">
-        <v>251</v>
-      </c>
-      <c r="E70" t="s">
-        <v>252</v>
-      </c>
-      <c r="F70" t="s">
-        <v>278</v>
       </c>
       <c r="G70" t="s">
         <v>13</v>
@@ -3114,22 +3098,19 @@
     </row>
     <row r="71" spans="1:7">
       <c r="A71" t="s">
+        <v>277</v>
+      </c>
+      <c r="B71" t="s">
+        <v>278</v>
+      </c>
+      <c r="C71" t="s">
+        <v>25</v>
+      </c>
+      <c r="E71" t="s">
+        <v>247</v>
+      </c>
+      <c r="F71" t="s">
         <v>279</v>
-      </c>
-      <c r="B71" t="s">
-        <v>280</v>
-      </c>
-      <c r="C71" t="s">
-        <v>69</v>
-      </c>
-      <c r="D71" t="s">
-        <v>26</v>
-      </c>
-      <c r="E71" t="s">
-        <v>252</v>
-      </c>
-      <c r="F71" t="s">
-        <v>281</v>
       </c>
       <c r="G71" t="s">
         <v>13</v>
@@ -3137,19 +3118,22 @@
     </row>
     <row r="72" spans="1:7">
       <c r="A72" t="s">
+        <v>280</v>
+      </c>
+      <c r="B72" t="s">
+        <v>281</v>
+      </c>
+      <c r="C72" t="s">
+        <v>34</v>
+      </c>
+      <c r="D72" t="s">
+        <v>177</v>
+      </c>
+      <c r="E72" t="s">
+        <v>247</v>
+      </c>
+      <c r="F72" t="s">
         <v>282</v>
-      </c>
-      <c r="B72" t="s">
-        <v>283</v>
-      </c>
-      <c r="C72" t="s">
-        <v>25</v>
-      </c>
-      <c r="E72" t="s">
-        <v>252</v>
-      </c>
-      <c r="F72" t="s">
-        <v>284</v>
       </c>
       <c r="G72" t="s">
         <v>13</v>
@@ -3157,22 +3141,22 @@
     </row>
     <row r="73" spans="1:7">
       <c r="A73" t="s">
+        <v>283</v>
+      </c>
+      <c r="B73" t="s">
+        <v>284</v>
+      </c>
+      <c r="C73" t="s">
         <v>285</v>
       </c>
-      <c r="B73" t="s">
-        <v>286</v>
-      </c>
-      <c r="C73" t="s">
-        <v>34</v>
-      </c>
       <c r="D73" t="s">
-        <v>182</v>
+        <v>151</v>
       </c>
       <c r="E73" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="F73" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="G73" t="s">
         <v>13</v>
@@ -3180,65 +3164,62 @@
     </row>
     <row r="74" spans="1:7">
       <c r="A74" t="s">
+        <v>286</v>
+      </c>
+      <c r="B74" t="s">
+        <v>287</v>
+      </c>
+      <c r="C74" t="s">
+        <v>25</v>
+      </c>
+      <c r="E74" t="s">
+        <v>247</v>
+      </c>
+      <c r="F74" t="s">
         <v>288</v>
       </c>
-      <c r="B74" t="s">
+      <c r="G74" t="s">
         <v>289</v>
-      </c>
-      <c r="C74" t="s">
-        <v>290</v>
-      </c>
-      <c r="D74" t="s">
-        <v>156</v>
-      </c>
-      <c r="E74" t="s">
-        <v>252</v>
-      </c>
-      <c r="F74" t="s">
-        <v>284</v>
-      </c>
-      <c r="G74" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="75" spans="1:7">
       <c r="A75" t="s">
+        <v>290</v>
+      </c>
+      <c r="B75" t="s">
         <v>291</v>
       </c>
-      <c r="B75" t="s">
+      <c r="C75" t="s">
         <v>292</v>
       </c>
-      <c r="C75" t="s">
-        <v>25</v>
+      <c r="D75" t="s">
+        <v>151</v>
       </c>
       <c r="E75" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="F75" t="s">
         <v>293</v>
       </c>
       <c r="G75" t="s">
-        <v>294</v>
+        <v>13</v>
       </c>
     </row>
     <row r="76" spans="1:7">
       <c r="A76" t="s">
+        <v>294</v>
+      </c>
+      <c r="B76" t="s">
         <v>295</v>
       </c>
-      <c r="B76" t="s">
+      <c r="C76" t="s">
+        <v>64</v>
+      </c>
+      <c r="E76" t="s">
+        <v>247</v>
+      </c>
+      <c r="F76" t="s">
         <v>296</v>
-      </c>
-      <c r="C76" t="s">
-        <v>297</v>
-      </c>
-      <c r="D76" t="s">
-        <v>156</v>
-      </c>
-      <c r="E76" t="s">
-        <v>252</v>
-      </c>
-      <c r="F76" t="s">
-        <v>298</v>
       </c>
       <c r="G76" t="s">
         <v>13</v>
@@ -3246,19 +3227,19 @@
     </row>
     <row r="77" spans="1:7">
       <c r="A77" t="s">
+        <v>297</v>
+      </c>
+      <c r="B77" t="s">
+        <v>298</v>
+      </c>
+      <c r="C77" t="s">
+        <v>268</v>
+      </c>
+      <c r="E77" t="s">
+        <v>247</v>
+      </c>
+      <c r="F77" t="s">
         <v>299</v>
-      </c>
-      <c r="B77" t="s">
-        <v>300</v>
-      </c>
-      <c r="C77" t="s">
-        <v>69</v>
-      </c>
-      <c r="E77" t="s">
-        <v>252</v>
-      </c>
-      <c r="F77" t="s">
-        <v>301</v>
       </c>
       <c r="G77" t="s">
         <v>13</v>
@@ -3266,19 +3247,22 @@
     </row>
     <row r="78" spans="1:7">
       <c r="A78" t="s">
+        <v>300</v>
+      </c>
+      <c r="B78" t="s">
+        <v>301</v>
+      </c>
+      <c r="C78" t="s">
+        <v>268</v>
+      </c>
+      <c r="D78" t="s">
+        <v>177</v>
+      </c>
+      <c r="E78" t="s">
+        <v>247</v>
+      </c>
+      <c r="F78" t="s">
         <v>302</v>
-      </c>
-      <c r="B78" t="s">
-        <v>303</v>
-      </c>
-      <c r="C78" t="s">
-        <v>273</v>
-      </c>
-      <c r="E78" t="s">
-        <v>252</v>
-      </c>
-      <c r="F78" t="s">
-        <v>304</v>
       </c>
       <c r="G78" t="s">
         <v>13</v>
@@ -3286,22 +3270,19 @@
     </row>
     <row r="79" spans="1:7">
       <c r="A79" t="s">
+        <v>303</v>
+      </c>
+      <c r="B79" t="s">
+        <v>304</v>
+      </c>
+      <c r="C79" t="s">
+        <v>39</v>
+      </c>
+      <c r="E79" t="s">
+        <v>247</v>
+      </c>
+      <c r="F79" t="s">
         <v>305</v>
-      </c>
-      <c r="B79" t="s">
-        <v>306</v>
-      </c>
-      <c r="C79" t="s">
-        <v>273</v>
-      </c>
-      <c r="D79" t="s">
-        <v>182</v>
-      </c>
-      <c r="E79" t="s">
-        <v>252</v>
-      </c>
-      <c r="F79" t="s">
-        <v>307</v>
       </c>
       <c r="G79" t="s">
         <v>13</v>
@@ -3309,19 +3290,22 @@
     </row>
     <row r="80" spans="1:7">
       <c r="A80" t="s">
+        <v>306</v>
+      </c>
+      <c r="B80" t="s">
+        <v>307</v>
+      </c>
+      <c r="C80" t="s">
+        <v>268</v>
+      </c>
+      <c r="D80" t="s">
+        <v>151</v>
+      </c>
+      <c r="E80" t="s">
+        <v>247</v>
+      </c>
+      <c r="F80" t="s">
         <v>308</v>
-      </c>
-      <c r="B80" t="s">
-        <v>309</v>
-      </c>
-      <c r="C80" t="s">
-        <v>39</v>
-      </c>
-      <c r="E80" t="s">
-        <v>252</v>
-      </c>
-      <c r="F80" t="s">
-        <v>310</v>
       </c>
       <c r="G80" t="s">
         <v>13</v>
@@ -3329,22 +3313,22 @@
     </row>
     <row r="81" spans="1:7">
       <c r="A81" t="s">
+        <v>309</v>
+      </c>
+      <c r="B81" t="s">
+        <v>310</v>
+      </c>
+      <c r="C81" t="s">
+        <v>292</v>
+      </c>
+      <c r="D81" t="s">
+        <v>151</v>
+      </c>
+      <c r="E81" t="s">
+        <v>247</v>
+      </c>
+      <c r="F81" t="s">
         <v>311</v>
-      </c>
-      <c r="B81" t="s">
-        <v>312</v>
-      </c>
-      <c r="C81" t="s">
-        <v>273</v>
-      </c>
-      <c r="D81" t="s">
-        <v>156</v>
-      </c>
-      <c r="E81" t="s">
-        <v>252</v>
-      </c>
-      <c r="F81" t="s">
-        <v>313</v>
       </c>
       <c r="G81" t="s">
         <v>13</v>
@@ -3352,22 +3336,22 @@
     </row>
     <row r="82" spans="1:7">
       <c r="A82" t="s">
+        <v>312</v>
+      </c>
+      <c r="B82" t="s">
+        <v>313</v>
+      </c>
+      <c r="C82" t="s">
+        <v>292</v>
+      </c>
+      <c r="D82" t="s">
+        <v>151</v>
+      </c>
+      <c r="E82" t="s">
+        <v>247</v>
+      </c>
+      <c r="F82" t="s">
         <v>314</v>
-      </c>
-      <c r="B82" t="s">
-        <v>315</v>
-      </c>
-      <c r="C82" t="s">
-        <v>297</v>
-      </c>
-      <c r="D82" t="s">
-        <v>156</v>
-      </c>
-      <c r="E82" t="s">
-        <v>252</v>
-      </c>
-      <c r="F82" t="s">
-        <v>316</v>
       </c>
       <c r="G82" t="s">
         <v>13</v>
@@ -3375,22 +3359,22 @@
     </row>
     <row r="83" spans="1:7">
       <c r="A83" t="s">
+        <v>315</v>
+      </c>
+      <c r="B83" t="s">
+        <v>316</v>
+      </c>
+      <c r="C83" t="s">
+        <v>34</v>
+      </c>
+      <c r="D83" t="s">
+        <v>151</v>
+      </c>
+      <c r="E83" t="s">
+        <v>247</v>
+      </c>
+      <c r="F83" t="s">
         <v>317</v>
-      </c>
-      <c r="B83" t="s">
-        <v>318</v>
-      </c>
-      <c r="C83" t="s">
-        <v>297</v>
-      </c>
-      <c r="D83" t="s">
-        <v>156</v>
-      </c>
-      <c r="E83" t="s">
-        <v>252</v>
-      </c>
-      <c r="F83" t="s">
-        <v>319</v>
       </c>
       <c r="G83" t="s">
         <v>13</v>
@@ -3398,22 +3382,22 @@
     </row>
     <row r="84" spans="1:7">
       <c r="A84" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B84" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C84" t="s">
         <v>34</v>
       </c>
       <c r="D84" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E84" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="F84" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="G84" t="s">
         <v>13</v>
@@ -3421,22 +3405,22 @@
     </row>
     <row r="85" spans="1:7">
       <c r="A85" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B85" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C85" t="s">
         <v>34</v>
       </c>
       <c r="D85" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E85" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="F85" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="G85" t="s">
         <v>13</v>
@@ -3444,22 +3428,22 @@
     </row>
     <row r="86" spans="1:7">
       <c r="A86" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B86" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C86" t="s">
         <v>34</v>
       </c>
       <c r="D86" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E86" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="F86" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G86" t="s">
         <v>13</v>
@@ -3467,19 +3451,19 @@
     </row>
     <row r="87" spans="1:7">
       <c r="A87" t="s">
+        <v>327</v>
+      </c>
+      <c r="B87" t="s">
+        <v>328</v>
+      </c>
+      <c r="C87" t="s">
         <v>329</v>
       </c>
-      <c r="B87" t="s">
+      <c r="D87" t="s">
         <v>330</v>
       </c>
-      <c r="C87" t="s">
-        <v>34</v>
-      </c>
-      <c r="D87" t="s">
-        <v>156</v>
-      </c>
       <c r="E87" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="F87" t="s">
         <v>331</v>
@@ -3502,7 +3486,7 @@
         <v>335</v>
       </c>
       <c r="E88" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="F88" t="s">
         <v>336</v>
@@ -3519,16 +3503,13 @@
         <v>338</v>
       </c>
       <c r="C89" t="s">
+        <v>39</v>
+      </c>
+      <c r="E89" t="s">
+        <v>247</v>
+      </c>
+      <c r="F89" t="s">
         <v>339</v>
-      </c>
-      <c r="D89" t="s">
-        <v>340</v>
-      </c>
-      <c r="E89" t="s">
-        <v>252</v>
-      </c>
-      <c r="F89" t="s">
-        <v>341</v>
       </c>
       <c r="G89" t="s">
         <v>13</v>
@@ -3536,19 +3517,22 @@
     </row>
     <row r="90" spans="1:7">
       <c r="A90" t="s">
+        <v>340</v>
+      </c>
+      <c r="B90" t="s">
+        <v>341</v>
+      </c>
+      <c r="C90" t="s">
+        <v>190</v>
+      </c>
+      <c r="D90" t="s">
         <v>342</v>
       </c>
-      <c r="B90" t="s">
+      <c r="E90" t="s">
+        <v>247</v>
+      </c>
+      <c r="F90" t="s">
         <v>343</v>
-      </c>
-      <c r="C90" t="s">
-        <v>39</v>
-      </c>
-      <c r="E90" t="s">
-        <v>252</v>
-      </c>
-      <c r="F90" t="s">
-        <v>344</v>
       </c>
       <c r="G90" t="s">
         <v>13</v>
@@ -3556,22 +3540,22 @@
     </row>
     <row r="91" spans="1:7">
       <c r="A91" t="s">
+        <v>344</v>
+      </c>
+      <c r="B91" t="s">
         <v>345</v>
       </c>
-      <c r="B91" t="s">
+      <c r="C91" t="s">
+        <v>39</v>
+      </c>
+      <c r="D91" t="s">
+        <v>26</v>
+      </c>
+      <c r="E91" t="s">
+        <v>247</v>
+      </c>
+      <c r="F91" t="s">
         <v>346</v>
-      </c>
-      <c r="C91" t="s">
-        <v>195</v>
-      </c>
-      <c r="D91" t="s">
-        <v>347</v>
-      </c>
-      <c r="E91" t="s">
-        <v>252</v>
-      </c>
-      <c r="F91" t="s">
-        <v>348</v>
       </c>
       <c r="G91" t="s">
         <v>13</v>
@@ -3579,22 +3563,19 @@
     </row>
     <row r="92" spans="1:7">
       <c r="A92" t="s">
+        <v>347</v>
+      </c>
+      <c r="B92" t="s">
+        <v>348</v>
+      </c>
+      <c r="C92" t="s">
         <v>349</v>
       </c>
-      <c r="B92" t="s">
+      <c r="E92" t="s">
+        <v>247</v>
+      </c>
+      <c r="F92" t="s">
         <v>350</v>
-      </c>
-      <c r="C92" t="s">
-        <v>39</v>
-      </c>
-      <c r="D92" t="s">
-        <v>26</v>
-      </c>
-      <c r="E92" t="s">
-        <v>252</v>
-      </c>
-      <c r="F92" t="s">
-        <v>351</v>
       </c>
       <c r="G92" t="s">
         <v>13</v>
@@ -3602,41 +3583,21 @@
     </row>
     <row r="93" spans="1:7">
       <c r="A93" t="s">
+        <v>351</v>
+      </c>
+      <c r="B93" t="s">
         <v>352</v>
       </c>
-      <c r="B93" t="s">
+      <c r="C93" t="s">
         <v>353</v>
       </c>
-      <c r="C93" t="s">
+      <c r="E93" t="s">
+        <v>247</v>
+      </c>
+      <c r="F93" t="s">
         <v>354</v>
       </c>
-      <c r="E93" t="s">
-        <v>252</v>
-      </c>
-      <c r="F93" t="s">
-        <v>355</v>
-      </c>
       <c r="G93" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7">
-      <c r="A94" t="s">
-        <v>356</v>
-      </c>
-      <c r="B94" t="s">
-        <v>357</v>
-      </c>
-      <c r="C94" t="s">
-        <v>358</v>
-      </c>
-      <c r="E94" t="s">
-        <v>252</v>
-      </c>
-      <c r="F94" t="s">
-        <v>359</v>
-      </c>
-      <c r="G94" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>